<commit_message>
excel parser for refactoring in main
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="9435" windowHeight="11760"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="9435" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="2" r:id="rId1"/>
-    <sheet name="autentification" sheetId="1" r:id="rId2"/>
-    <sheet name="message" sheetId="3" r:id="rId3"/>
+    <sheet name="autentification1" sheetId="1" r:id="rId2"/>
+    <sheet name="autentification" sheetId="4" r:id="rId3"/>
+    <sheet name="message" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="data" localSheetId="1">autentification!$A$2:$D$4</definedName>
+    <definedName name="data" localSheetId="1">autentification1!$A$2:$D$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>AutentificationSuccessful</t>
   </si>
@@ -76,6 +77,9 @@
   </si>
   <si>
     <t>data</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -269,8 +273,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -575,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -586,13 +590,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -600,7 +604,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -608,7 +612,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -633,7 +637,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,6 +732,90 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="test.auto.lab@gmail.com"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add  input data for messages
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -8,16 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="2" r:id="rId1"/>
-    <sheet name="autentification1" sheetId="1" r:id="rId2"/>
-    <sheet name="autentification" sheetId="4" r:id="rId3"/>
-    <sheet name="message" sheetId="3" r:id="rId4"/>
+    <sheet name="autentification" sheetId="4" r:id="rId2"/>
+    <sheet name="message" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>AutentificationSuccessful</t>
   </si>
@@ -25,9 +24,6 @@
     <t>AutentificationWithInvalidPassword</t>
   </si>
   <si>
-    <t>LogoutSuccessfull</t>
-  </si>
-  <si>
     <t>Parameter1</t>
   </si>
   <si>
@@ -73,20 +69,47 @@
     <t>Password</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>LogoutSuccessful</t>
+  </si>
+  <si>
+    <t>SendTextMessage</t>
+  </si>
+  <si>
+    <t>SendMessageWithIncorrectEmail</t>
+  </si>
+  <si>
+    <t>SendMessageWithEmptyEmail</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>some text</t>
+  </si>
+  <si>
+    <t>Parameter4</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>incorrect_email</t>
+  </si>
+  <si>
+    <t>ErrorThe address \"incorrect_email\" in the \"To\" field was not recognized. Please make sure that all addresses are properly formed.</t>
+  </si>
+  <si>
+    <t>ErrorPlease specify at least one recipient.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +141,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,8 +216,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -227,20 +269,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -248,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -269,12 +304,54 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -580,7 +657,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,33 +667,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="16"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="19"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="B3" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>17</v>
-      </c>
       <c r="B4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -634,108 +711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="15"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="test.auto.lab@gmail.com"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4"/>
-    <hyperlink ref="D2" r:id="rId5"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,16 +727,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -765,13 +744,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -779,27 +758,27 @@
         <v>1</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -814,14 +793,90 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="22" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add logger and attach
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="9435" windowHeight="11760"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="9435" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="global" sheetId="2" r:id="rId1"/>
@@ -306,7 +306,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -352,6 +351,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -656,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -667,10 +667,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,7 +798,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,68 +810,68 @@
     <col min="5" max="5" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="22" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:5" s="21" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:5" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>